<commit_message>
smoke test cases done
</commit_message>
<xml_diff>
--- a/smoke_cycle.xlsx
+++ b/smoke_cycle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University_Study\Final Year Project\FYP-2\Project\Project-final\TourToPk\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University_Study\Final Year Project\FYP-2\Project\TourToPK-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E078257B-270A-4575-BD24-4B5D90EF66C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E909B7-7FD5-4153-97B5-3F6AD51BD717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5AB937BA-5FA4-4948-8E51-9C0E50EACC05}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t xml:space="preserve">Functionality </t>
   </si>
@@ -228,6 +228,63 @@
   </si>
   <si>
     <t>able to naviage to all pages</t>
+  </si>
+  <si>
+    <t>Able to navigate all links</t>
+  </si>
+  <si>
+    <t>able to view and delete plans</t>
+  </si>
+  <si>
+    <t>able to view and delete places</t>
+  </si>
+  <si>
+    <t>TourToPK Dashboard</t>
+  </si>
+  <si>
+    <t>able to view and delete hotels</t>
+  </si>
+  <si>
+    <t>able to view and delete packages</t>
+  </si>
+  <si>
+    <t>able to create partners accounts</t>
+  </si>
+  <si>
+    <t>Content Manager
+dashboad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">able to navigate all links </t>
+  </si>
+  <si>
+    <t>able to create, update, delete places</t>
+  </si>
+  <si>
+    <t>abe to create,update,delete plans</t>
+  </si>
+  <si>
+    <t>able to view and delete all tourists</t>
+  </si>
+  <si>
+    <t>Hotel Manger 
+dahsboard</t>
+  </si>
+  <si>
+    <t>able to naviage all links</t>
+  </si>
+  <si>
+    <t>able to create, update, delete hotels</t>
+  </si>
+  <si>
+    <t>able to view and delete booking</t>
+  </si>
+  <si>
+    <t>Tour Operator 
+dashboard</t>
+  </si>
+  <si>
+    <t>able to create, update, delete packages</t>
   </si>
 </sst>
 </file>
@@ -624,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9112D2C2-6ECA-4DE2-82FD-50F89D5E6DF6}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,14 +1041,141 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
       <c r="C33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C33" xr:uid="{8361DD56-0BCB-42B6-AB29-4ED010D7023B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C47" xr:uid="{8361DD56-0BCB-42B6-AB29-4ED010D7023B}">
       <formula1>"PASS, FAIL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>